<commit_message>
reorganized everything, finished assignment
</commit_message>
<xml_diff>
--- a/Julia times.xlsx
+++ b/Julia times.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>p</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>wobbie</t>
+  </si>
+  <si>
+    <t>efficiency</t>
   </si>
 </sst>
 </file>
@@ -128,14 +131,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -152,6 +149,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,6 +165,421 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>julia_omp: Threaded Speedup</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>julia_omp</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6578947368421053</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7027027027027026</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8461538461538458</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:hiLowLines/>
+        <c:marker val="1"/>
+        <c:axId val="80460032"/>
+        <c:axId val="80470016"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="80460032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80470016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="80470016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relative Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80460032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>julia_omp: Threaded Efficiency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>julia_omp</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82894736842105265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42567567567567566</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.328125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30288461538461536</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:hiLowLines/>
+        <c:marker val="1"/>
+        <c:axId val="82712064"/>
+        <c:axId val="141378688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="82712064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Numer of Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141378688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="141378688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relative Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82712064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>643890</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>643890</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -446,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -457,41 +878,44 @@
     <col min="1" max="1" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="2"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4"/>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="2"/>
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="H2" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3">
@@ -508,10 +932,14 @@
         <f>$E$3/E3</f>
         <v>1</v>
       </c>
+      <c r="H3">
+        <f>F3/B3</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
-      <c r="B4" s="7">
+    <row r="4" spans="1:8">
+      <c r="A4" s="10"/>
+      <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4">
@@ -528,10 +956,14 @@
         <f>$E$3/E4</f>
         <v>1.6578947368421053</v>
       </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H8" si="1">F4/B4</f>
+        <v>0.82894736842105265</v>
+      </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
-      <c r="B5" s="7">
+    <row r="5" spans="1:8">
+      <c r="A5" s="10"/>
+      <c r="B5" s="5">
         <v>4</v>
       </c>
       <c r="C5">
@@ -545,13 +977,17 @@
         <v>37</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F8" si="1">$E$3/E5</f>
+        <f t="shared" ref="F5:F8" si="2">$E$3/E5</f>
         <v>1.7027027027027026</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0.42567567567567566</v>
+      </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="7">
+    <row r="6" spans="1:8">
+      <c r="A6" s="10"/>
+      <c r="B6" s="5">
         <v>8</v>
       </c>
       <c r="C6">
@@ -565,13 +1001,17 @@
         <v>24</v>
       </c>
       <c r="F6">
+        <f t="shared" si="2"/>
+        <v>2.625</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="1"/>
-        <v>2.625</v>
+        <v>0.328125</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1"/>
-      <c r="B7" s="7">
+    <row r="7" spans="1:8">
+      <c r="A7" s="10"/>
+      <c r="B7" s="5">
         <v>16</v>
       </c>
       <c r="C7">
@@ -585,13 +1025,17 @@
         <v>13</v>
       </c>
       <c r="F7">
+        <f t="shared" si="2"/>
+        <v>4.8461538461538458</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="1"/>
-        <v>4.8461538461538458</v>
+        <v>0.30288461538461536</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
-      <c r="B8" s="7">
+    <row r="8" spans="1:8">
+      <c r="A8" s="10"/>
+      <c r="B8" s="5">
         <v>32</v>
       </c>
       <c r="C8">
@@ -605,39 +1049,43 @@
         <v>7</v>
       </c>
       <c r="F8">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0.28125</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="5">
+      <c r="B9" s="6"/>
+      <c r="C9" s="3">
         <v>0.88</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>59.090909090909093</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="5">
+      <c r="B10" s="6"/>
+      <c r="C10" s="3">
         <v>3.48</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>14.942528735632184</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -647,6 +1095,10 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CJulia Times</oddHeader>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
pdf of table and plts
</commit_message>
<xml_diff>
--- a/Julia times.xlsx
+++ b/Julia times.xlsx
@@ -149,14 +149,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -257,14 +257,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:hiLowLines/>
         <c:marker val="1"/>
-        <c:axId val="80460032"/>
-        <c:axId val="80470016"/>
+        <c:axId val="66936832"/>
+        <c:axId val="66977792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80460032"/>
+        <c:axId val="66936832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -290,14 +289,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80470016"/>
+        <c:crossAx val="66977792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80470016"/>
+        <c:axId val="66977792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -323,7 +322,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80460032"/>
+        <c:crossAx val="66936832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -336,7 +335,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -432,14 +431,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:hiLowLines/>
         <c:marker val="1"/>
-        <c:axId val="82712064"/>
-        <c:axId val="141378688"/>
+        <c:axId val="66988288"/>
+        <c:axId val="67146496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82712064"/>
+        <c:axId val="66988288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,14 +463,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141378688"/>
+        <c:crossAx val="67146496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141378688"/>
+        <c:axId val="67146496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -498,7 +496,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82712064"/>
+        <c:crossAx val="66988288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -511,7 +509,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -528,7 +526,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>643890</xdr:colOff>
+      <xdr:colOff>625602</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -558,7 +556,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>643890</xdr:colOff>
+      <xdr:colOff>625602</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -869,9 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -881,14 +877,14 @@
     <row r="1" spans="1:8">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2"/>
@@ -907,12 +903,12 @@
       <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5">
@@ -938,7 +934,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="10"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -962,7 +958,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="10"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="5">
         <v>4</v>
       </c>
@@ -986,7 +982,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="5">
         <v>8</v>
       </c>
@@ -1010,7 +1006,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="10"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="5">
         <v>16</v>
       </c>
@@ -1034,7 +1030,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="10"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="5">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
made julia_omp significantly faster, other updates
</commit_message>
<xml_diff>
--- a/Julia times.xlsx
+++ b/Julia times.xlsx
@@ -182,7 +182,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>julia_omp: Threaded Speedup</a:t>
+              <a:t>julia_omp:</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Threaded</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Speedup</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -239,19 +247,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6578947368421053</c:v>
+                  <c:v>2.1785702947917791</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7027027027027026</c:v>
+                  <c:v>3.5509181883566781</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.625</c:v>
+                  <c:v>6.7190874822538795</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8461538461538458</c:v>
+                  <c:v>11.139293517253021</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>15.277452503817951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -259,11 +267,11 @@
         </c:ser>
         <c:hiLowLines/>
         <c:marker val="1"/>
-        <c:axId val="66936832"/>
-        <c:axId val="66977792"/>
+        <c:axId val="127050112"/>
+        <c:axId val="127052032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66936832"/>
+        <c:axId val="127050112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -289,14 +297,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66977792"/>
+        <c:crossAx val="127052032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66977792"/>
+        <c:axId val="127052032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -313,8 +321,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Relative Speedup</a:t>
+                  <a:t>Relative</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Speedup</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -322,7 +335,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66936832"/>
+        <c:crossAx val="127050112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -335,7 +348,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -413,19 +426,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82894736842105265</c:v>
+                  <c:v>1.0892851473958896</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42567567567567566</c:v>
+                  <c:v>0.88772954708916951</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.328125</c:v>
+                  <c:v>0.83988593528173494</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.30288461538461536</c:v>
+                  <c:v>0.69620584482831382</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.28125</c:v>
+                  <c:v>0.47742039074431097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -433,11 +446,11 @@
         </c:ser>
         <c:hiLowLines/>
         <c:marker val="1"/>
-        <c:axId val="66988288"/>
-        <c:axId val="67146496"/>
+        <c:axId val="127347712"/>
+        <c:axId val="127366272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66988288"/>
+        <c:axId val="127347712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,7 +466,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Numer of Threads</a:t>
+                  <a:t>Number of Threads</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -463,14 +476,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67146496"/>
+        <c:crossAx val="127366272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67146496"/>
+        <c:axId val="127366272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +509,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66988288"/>
+        <c:crossAx val="127347712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -509,7 +522,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -522,13 +535,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>625602</xdr:colOff>
+      <xdr:colOff>643890</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -552,13 +565,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>625602</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -867,7 +880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -915,14 +930,14 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <f>$C$3/C3</f>
         <v>1</v>
       </c>
       <c r="E3">
-        <v>63</v>
+        <v>68.625399999999999</v>
       </c>
       <c r="F3">
         <f>$E$3/E3</f>
@@ -939,22 +954,22 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D10" si="0">$C$3/C4</f>
-        <v>1.625</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>38</v>
+        <v>31.5002</v>
       </c>
       <c r="F4">
         <f>$E$3/E4</f>
-        <v>1.6578947368421053</v>
+        <v>2.1785702947917791</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H8" si="1">F4/B4</f>
-        <v>0.82894736842105265</v>
+        <v>1.0892851473958896</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -963,22 +978,22 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1.6774193548387097</v>
+        <v>4.1428571428571432</v>
       </c>
       <c r="E5">
-        <v>37</v>
+        <v>19.3261</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F8" si="2">$E$3/E5</f>
-        <v>1.7027027027027026</v>
+        <v>3.5509181883566781</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>0.42567567567567566</v>
+        <v>0.88772954708916951</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -987,22 +1002,22 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>2.4761904761904763</v>
+        <v>8.2857142857142865</v>
       </c>
       <c r="E6">
-        <v>24</v>
+        <v>10.2135</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>2.625</v>
+        <v>6.7190874822538795</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>0.328125</v>
+        <v>0.83988593528173494</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1011,22 +1026,22 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>4.7272727272727275</v>
+        <v>8.2857142857142865</v>
       </c>
       <c r="E7">
-        <v>13</v>
+        <v>6.16066</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>4.8461538461538458</v>
+        <v>11.139293517253021</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>0.30288461538461536</v>
+        <v>0.69620584482831382</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1035,22 +1050,22 @@
         <v>32</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>8.2857142857142865</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>4.4919399999999996</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>15.277452503817951</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>0.28125</v>
+        <v>0.47742039074431097</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1063,7 +1078,7 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>59.090909090909093</v>
+        <v>65.909090909090907</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1078,7 +1093,7 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>14.942528735632184</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1102,11 +1117,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>